<commit_message>
Clarify cascading select example
</commit_message>
<xml_diff>
--- a/assets/xlsx/cascading_select.xlsx
+++ b/assets/xlsx/cascading_select.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>type</t>
   </si>
@@ -30,33 +30,45 @@
     <t>select_one states</t>
   </si>
   <si>
+    <t>selected_state</t>
+  </si>
+  <si>
+    <t>Select a state</t>
+  </si>
+  <si>
+    <t>select_one counties</t>
+  </si>
+  <si>
+    <t>selected_county</t>
+  </si>
+  <si>
+    <t>Select a county</t>
+  </si>
+  <si>
+    <t>state=${selected_state}</t>
+  </si>
+  <si>
+    <t>select_one cities</t>
+  </si>
+  <si>
+    <t>selected_city</t>
+  </si>
+  <si>
+    <t>Select a city</t>
+  </si>
+  <si>
+    <t>county=${selected_county}</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
     <t>state</t>
   </si>
   <si>
-    <t>select_one counties</t>
-  </si>
-  <si>
     <t>county</t>
   </si>
   <si>
-    <t>cf=${state}</t>
-  </si>
-  <si>
-    <t>select_one cities</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>cf=${county}</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>cf</t>
-  </si>
-  <si>
     <t>states</t>
   </si>
   <si>
@@ -102,18 +114,6 @@
     <t>cities</t>
   </si>
   <si>
-    <t>dumont</t>
-  </si>
-  <si>
-    <t>Dumont</t>
-  </si>
-  <si>
-    <t>finney</t>
-  </si>
-  <si>
-    <t>Finney</t>
-  </si>
-  <si>
     <t>brownsville</t>
   </si>
   <si>
@@ -156,7 +156,10 @@
     <t>form_id</t>
   </si>
   <si>
-    <t>cascading select test</t>
+    <t>Cascading select example</t>
+  </si>
+  <si>
+    <t>cascading_select</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1413,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1432,16 +1435,16 @@
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1462,16 +1465,16 @@
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" t="s" s="6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s" s="6">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s" s="6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1873,7 +1876,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s" s="6">
         <v>1</v>
@@ -1882,20 +1885,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="E1" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="E1" t="s" s="6">
+        <v>17</v>
+      </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s" s="6">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s" s="6">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1903,117 +1908,101 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s" s="6">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="6">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>17</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s" s="6">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s" s="6">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s" s="6">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s" s="6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s" s="6">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s" s="6">
         <v>19</v>
-      </c>
-      <c r="B7" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s" s="6">
-        <v>15</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" t="s" s="6">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s" s="6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s" s="6">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>20</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s" s="6">
         <v>33</v>
@@ -2022,14 +2011,16 @@
         <v>34</v>
       </c>
       <c r="D10" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E10" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="E10" t="s" s="6">
+        <v>30</v>
+      </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s" s="6">
         <v>35</v>
@@ -2038,14 +2029,16 @@
         <v>36</v>
       </c>
       <c r="D11" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E11" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="E11" t="s" s="6">
+        <v>30</v>
+      </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s" s="6">
         <v>37</v>
@@ -2054,14 +2047,16 @@
         <v>38</v>
       </c>
       <c r="D12" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E12" t="s" s="6">
+        <v>24</v>
+      </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s" s="6">
         <v>39</v>
@@ -2070,14 +2065,16 @@
         <v>40</v>
       </c>
       <c r="D13" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="E13" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E13" t="s" s="6">
+        <v>24</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s" s="6">
         <v>41</v>
@@ -2086,14 +2083,16 @@
         <v>42</v>
       </c>
       <c r="D14" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="E14" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E14" t="s" s="6">
+        <v>26</v>
+      </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s" s="6">
         <v>43</v>
@@ -2102,9 +2101,11 @@
         <v>44</v>
       </c>
       <c r="D15" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="E15" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E15" t="s" s="6">
+        <v>26</v>
+      </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" ht="13.65" customHeight="1">
@@ -2192,7 +2193,9 @@
       <c r="A2" t="s" s="6">
         <v>47</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" t="s" s="6">
+        <v>48</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>

</xml_diff>

<commit_message>
Clarify cascading select example (#207)
</commit_message>
<xml_diff>
--- a/assets/xlsx/cascading_select.xlsx
+++ b/assets/xlsx/cascading_select.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>type</t>
   </si>
@@ -30,33 +30,45 @@
     <t>select_one states</t>
   </si>
   <si>
+    <t>selected_state</t>
+  </si>
+  <si>
+    <t>Select a state</t>
+  </si>
+  <si>
+    <t>select_one counties</t>
+  </si>
+  <si>
+    <t>selected_county</t>
+  </si>
+  <si>
+    <t>Select a county</t>
+  </si>
+  <si>
+    <t>state=${selected_state}</t>
+  </si>
+  <si>
+    <t>select_one cities</t>
+  </si>
+  <si>
+    <t>selected_city</t>
+  </si>
+  <si>
+    <t>Select a city</t>
+  </si>
+  <si>
+    <t>county=${selected_county}</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
     <t>state</t>
   </si>
   <si>
-    <t>select_one counties</t>
-  </si>
-  <si>
     <t>county</t>
   </si>
   <si>
-    <t>cf=${state}</t>
-  </si>
-  <si>
-    <t>select_one cities</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>cf=${county}</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>cf</t>
-  </si>
-  <si>
     <t>states</t>
   </si>
   <si>
@@ -102,18 +114,6 @@
     <t>cities</t>
   </si>
   <si>
-    <t>dumont</t>
-  </si>
-  <si>
-    <t>Dumont</t>
-  </si>
-  <si>
-    <t>finney</t>
-  </si>
-  <si>
-    <t>Finney</t>
-  </si>
-  <si>
     <t>brownsville</t>
   </si>
   <si>
@@ -156,7 +156,10 @@
     <t>form_id</t>
   </si>
   <si>
-    <t>cascading select test</t>
+    <t>Cascading select example</t>
+  </si>
+  <si>
+    <t>cascading_select</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1413,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1432,16 +1435,16 @@
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1462,16 +1465,16 @@
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" t="s" s="6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s" s="6">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s" s="6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1873,7 +1876,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s" s="6">
         <v>1</v>
@@ -1882,20 +1885,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="E1" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="E1" t="s" s="6">
+        <v>17</v>
+      </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s" s="6">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s" s="6">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1903,117 +1908,101 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s" s="6">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="6">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>17</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s" s="6">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s" s="6">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s" s="6">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s" s="6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s" s="6">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s" s="6">
         <v>19</v>
-      </c>
-      <c r="B7" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s" s="6">
-        <v>15</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" t="s" s="6">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s" s="6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s" s="6">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>20</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s" s="6">
         <v>33</v>
@@ -2022,14 +2011,16 @@
         <v>34</v>
       </c>
       <c r="D10" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E10" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="E10" t="s" s="6">
+        <v>30</v>
+      </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s" s="6">
         <v>35</v>
@@ -2038,14 +2029,16 @@
         <v>36</v>
       </c>
       <c r="D11" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E11" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="E11" t="s" s="6">
+        <v>30</v>
+      </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s" s="6">
         <v>37</v>
@@ -2054,14 +2047,16 @@
         <v>38</v>
       </c>
       <c r="D12" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E12" t="s" s="6">
+        <v>24</v>
+      </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s" s="6">
         <v>39</v>
@@ -2070,14 +2065,16 @@
         <v>40</v>
       </c>
       <c r="D13" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="E13" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E13" t="s" s="6">
+        <v>24</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s" s="6">
         <v>41</v>
@@ -2086,14 +2083,16 @@
         <v>42</v>
       </c>
       <c r="D14" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="E14" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E14" t="s" s="6">
+        <v>26</v>
+      </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s" s="6">
         <v>43</v>
@@ -2102,9 +2101,11 @@
         <v>44</v>
       </c>
       <c r="D15" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="E15" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E15" t="s" s="6">
+        <v>26</v>
+      </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" ht="13.65" customHeight="1">
@@ -2192,7 +2193,9 @@
       <c r="A2" t="s" s="6">
         <v>47</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" t="s" s="6">
+        <v>48</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>

</xml_diff>